<commit_message>
Put code that fixes common mistakes in the raw data
</commit_message>
<xml_diff>
--- a/input/SCCWRP_SWAMP_FieldDataSheet.xlsx
+++ b/input/SCCWRP_SWAMP_FieldDataSheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/itlender/Projects/BLM_data_reformatter/input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://adcsuf-my.sharepoint.com/personal/duynguyen1993_csu_fullerton_edu/Documents/Work-Related Documents/SCCWRP/Projects/BLM_data_reformatter/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA55B82-4FFE-704E-84DB-909FE59963FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7DA55B82-4FFE-704E-84DB-909FE59963FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F9992A9-CA6A-49D9-BF3B-E2F7A1163B99}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2640" yWindow="2505" windowWidth="18165" windowHeight="14040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sccwrp_swamp_fielddatasheet_0" sheetId="2" r:id="rId1"/>
@@ -2384,329 +2384,329 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="16" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="16" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="12" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="55.83203125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="14" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="11" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="23" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="84" max="85" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="84" max="85" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="100" max="100" width="23" bestFit="1" customWidth="1"/>
-    <col min="101" max="101" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="103" max="103" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="104" max="104" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="106" max="106" width="19" bestFit="1" customWidth="1"/>
-    <col min="107" max="107" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="113" max="113" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="80.5" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="80.42578125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="119" max="119" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="121" max="121" width="120" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="124" max="124" width="13" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="127" max="127" width="10" bestFit="1" customWidth="1"/>
     <col min="128" max="128" width="13" bestFit="1" customWidth="1"/>
-    <col min="129" max="129" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="130" max="130" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="132" max="132" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="136" max="136" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="137" max="137" width="106.1640625" bestFit="1" customWidth="1"/>
-    <col min="138" max="138" width="50.1640625" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="130" max="130" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="133" max="133" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="137" max="137" width="106.140625" bestFit="1" customWidth="1"/>
+    <col min="138" max="138" width="50.140625" bestFit="1" customWidth="1"/>
     <col min="139" max="139" width="23" bestFit="1" customWidth="1"/>
-    <col min="140" max="140" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="140" max="140" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="141" max="141" width="24" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="28.6640625" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="143" max="143" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="144" max="144" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="145" max="145" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="146" max="146" width="13" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="148" max="148" width="12" bestFit="1" customWidth="1"/>
-    <col min="149" max="149" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="151" max="151" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="152" max="152" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="149" max="149" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="152" max="152" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="153" max="153" width="20" bestFit="1" customWidth="1"/>
-    <col min="154" max="154" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="155" max="155" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="156" max="156" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="157" max="157" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="159" max="159" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="161" max="161" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="162" max="162" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="163" max="163" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="164" max="164" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="171" max="172" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="173" max="173" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="174" max="174" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="176" max="176" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="177" max="177" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="178" max="178" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="181" max="182" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="191" max="192" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="195" max="195" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="196" max="196" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="200" max="200" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="201" max="202" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="24.83203125" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="205" max="205" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="207" max="207" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="209" max="209" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="210" max="210" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="211" max="212" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="213" max="213" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="154" max="154" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="155" max="155" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="156" max="156" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="157" max="157" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="158" max="158" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="159" max="159" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="163" max="163" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="164" max="164" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="165" max="165" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="166" max="166" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="167" max="167" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="168" max="168" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="169" max="169" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="170" max="170" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="171" max="172" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="173" max="173" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="174" max="174" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="176" max="176" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="177" max="177" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="178" max="178" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="179" max="179" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="181" max="182" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="183" max="183" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="190" max="190" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="191" max="192" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="193" max="193" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="200" max="200" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="201" max="202" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="205" max="205" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="206" max="206" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="207" max="207" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="209" max="209" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="210" max="210" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="211" max="212" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="213" max="213" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="214" max="214" width="21" bestFit="1" customWidth="1"/>
-    <col min="215" max="215" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="215" max="215" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="216" max="216" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="217" max="217" width="19" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="219" max="219" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="220" max="220" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="219" max="219" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="220" max="220" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="221" max="221" width="21" bestFit="1" customWidth="1"/>
-    <col min="222" max="222" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="225" max="225" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="230" max="230" width="19" bestFit="1" customWidth="1"/>
     <col min="231" max="231" width="20" bestFit="1" customWidth="1"/>
     <col min="232" max="232" width="8" bestFit="1" customWidth="1"/>
-    <col min="233" max="233" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="234" max="234" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="235" max="235" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="237" max="237" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="239" max="239" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="240" max="240" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="233" max="233" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="234" max="234" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="235" max="235" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="236" max="236" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="237" max="237" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="239" max="239" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="240" max="240" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="241" max="241" width="18" bestFit="1" customWidth="1"/>
-    <col min="242" max="242" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="243" max="243" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="244" max="244" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="245" max="245" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="246" max="246" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="242" max="242" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="243" max="243" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="244" max="244" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="245" max="245" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="246" max="246" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="247" max="247" width="13" bestFit="1" customWidth="1"/>
-    <col min="248" max="248" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="249" max="249" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="250" max="250" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="252" max="252" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="253" max="253" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="248" max="248" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="249" max="249" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="250" max="250" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="251" max="251" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="252" max="252" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="253" max="253" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="254" max="254" width="22" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="43.5" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="256" max="256" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="260" max="260" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="261" max="261" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="262" max="262" width="21" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="265" max="265" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="267" max="267" width="28" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="269" max="269" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="268" max="268" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="272" max="272" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="273" max="273" width="17" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="275" max="275" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="274" max="274" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="275" max="275" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="276" max="276" width="18" bestFit="1" customWidth="1"/>
     <col min="277" max="277" width="16" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="279" max="279" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="280" max="280" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="281" max="281" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="279" max="279" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="281" max="281" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="282" max="282" width="14" bestFit="1" customWidth="1"/>
-    <col min="283" max="283" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="284" max="284" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="285" max="285" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="286" max="286" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="283" max="283" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="284" max="284" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="285" max="285" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="286" max="286" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="287" max="287" width="23" bestFit="1" customWidth="1"/>
-    <col min="288" max="288" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="288" max="288" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="289" max="289" width="17" bestFit="1" customWidth="1"/>
-    <col min="290" max="290" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="291" max="291" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="290" max="290" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="291" max="291" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="292" max="292" width="18" bestFit="1" customWidth="1"/>
-    <col min="293" max="293" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="294" max="294" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="295" max="295" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="296" max="296" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="293" max="293" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="294" max="294" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="295" max="295" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="296" max="296" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="297" max="297" width="23" bestFit="1" customWidth="1"/>
-    <col min="298" max="298" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="299" max="299" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="298" max="298" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="299" max="299" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="300" max="300" width="24" bestFit="1" customWidth="1"/>
-    <col min="301" max="301" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="302" max="302" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="301" max="301" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="302" max="302" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="303" max="303" width="29" bestFit="1" customWidth="1"/>
-    <col min="304" max="304" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="304" max="304" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="305" max="305" width="26" bestFit="1" customWidth="1"/>
-    <col min="306" max="306" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="307" max="307" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="308" max="308" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="309" max="309" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="306" max="306" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="307" max="307" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="308" max="308" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="309" max="309" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="310" max="310" width="18" bestFit="1" customWidth="1"/>
-    <col min="311" max="311" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="312" max="312" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="313" max="313" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="314" max="314" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="311" max="311" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="312" max="312" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="313" max="313" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="314" max="314" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="315" max="315" width="26" bestFit="1" customWidth="1"/>
-    <col min="316" max="316" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="317" max="317" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="318" max="318" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="319" max="319" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="320" max="320" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="321" max="321" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="322" max="322" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="323" max="323" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="324" max="324" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="325" max="325" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="326" max="326" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="327" max="327" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="316" max="316" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="317" max="317" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="318" max="318" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="319" max="319" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="320" max="320" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="321" max="321" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="322" max="322" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="323" max="323" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="324" max="324" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="325" max="325" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="326" max="326" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="327" max="327" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3689,7 +3689,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="2" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>9</v>
       </c>
@@ -4432,7 +4432,7 @@
         <v>32.834206500000001</v>
       </c>
     </row>
-    <row r="3" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -5226,7 +5226,7 @@
         <v>32.820357000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>11</v>
       </c>
@@ -6026,7 +6026,7 @@
         <v>32.793138499999998</v>
       </c>
     </row>
-    <row r="5" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>12</v>
       </c>
@@ -6820,7 +6820,7 @@
         <v>32.781503999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13</v>
       </c>
@@ -7539,7 +7539,7 @@
         <v>32.772347166666698</v>
       </c>
     </row>
-    <row r="7" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>14</v>
       </c>
@@ -8267,7 +8267,7 @@
         <v>32.783835166666698</v>
       </c>
     </row>
-    <row r="8" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15</v>
       </c>
@@ -9133,7 +9133,7 @@
         <v>33.989431000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>16</v>
       </c>
@@ -9990,7 +9990,7 @@
         <v>34.038508999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>17</v>
       </c>
@@ -10748,7 +10748,7 @@
         <v>34.038837000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>18</v>
       </c>
@@ -11584,7 +11584,7 @@
         <v>34.022413833333303</v>
       </c>
     </row>
-    <row r="12" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>19</v>
       </c>
@@ -12360,7 +12360,7 @@
         <v>33.9938893333333</v>
       </c>
     </row>
-    <row r="13" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20</v>
       </c>
@@ -12938,7 +12938,7 @@
         <v>33.929567833333302</v>
       </c>
     </row>
-    <row r="14" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>21</v>
       </c>
@@ -13768,7 +13768,7 @@
         <v>33.870953166666702</v>
       </c>
     </row>
-    <row r="15" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>22</v>
       </c>
@@ -14598,7 +14598,7 @@
         <v>33.794215000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>23</v>
       </c>
@@ -15479,7 +15479,7 @@
         <v>33.989436833333301</v>
       </c>
     </row>
-    <row r="17" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>24</v>
       </c>
@@ -16333,7 +16333,7 @@
         <v>34.038637000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>25</v>
       </c>
@@ -17124,7 +17124,7 @@
         <v>34.038840833333303</v>
       </c>
     </row>
-    <row r="19" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>26</v>
       </c>
@@ -17717,7 +17717,7 @@
         <v>33.993962500000002</v>
       </c>
     </row>
-    <row r="20" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>27</v>
       </c>
@@ -18307,7 +18307,7 @@
         <v>33.929560833333298</v>
       </c>
     </row>
-    <row r="21" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>28</v>
       </c>
@@ -19143,7 +19143,7 @@
         <v>33.870972666666702</v>
       </c>
     </row>
-    <row r="22" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>29</v>
       </c>
@@ -19982,7 +19982,7 @@
         <v>33.791037666666703</v>
       </c>
     </row>
-    <row r="23" spans="1:327" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:327" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>30</v>
       </c>

</xml_diff>